<commit_message>
mudança critica, volte antes disso aqui, novo setup para uso coletivo
</commit_message>
<xml_diff>
--- a/backend/consumo_diario.xlsx
+++ b/backend/consumo_diario.xlsx
@@ -378,7 +378,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1147.61</v>
+        <v>1070.5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -387,16 +387,16 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>720</v>
+        <v>144</v>
       </c>
       <c r="F2">
-        <v>3570.7</v>
+        <v>3652.23</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>5438.3099999999995</v>
+        <v>4866.73</v>
       </c>
     </row>
     <row r="3">
@@ -404,7 +404,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1156.68</v>
+        <v>1129.46</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -413,16 +413,16 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>720</v>
+        <v>288</v>
       </c>
       <c r="F3">
-        <v>3608.83</v>
+        <v>3693.63</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
-        <v>5485.51</v>
+        <v>5111.09</v>
       </c>
     </row>
     <row r="4">
@@ -430,25 +430,25 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1111.32</v>
+        <v>1165.75</v>
       </c>
       <c r="C4">
-        <v>123.2</v>
+        <v>82.64</v>
       </c>
       <c r="D4">
-        <v>130.2</v>
+        <v>128.86</v>
       </c>
       <c r="E4">
-        <v>864</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>3622.14</v>
+        <v>3581.92</v>
       </c>
       <c r="G4">
-        <v>14.6</v>
+        <v>3.39</v>
       </c>
       <c r="H4">
-        <v>5865.460000000001</v>
+        <v>4962.56</v>
       </c>
     </row>
     <row r="5">
@@ -456,25 +456,25 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1846.15</v>
+        <v>1687.39</v>
       </c>
       <c r="C5">
-        <v>1264.81</v>
+        <v>1198.18</v>
       </c>
       <c r="D5">
-        <v>1315.09</v>
+        <v>1443.77</v>
       </c>
       <c r="E5">
-        <v>1008</v>
+        <v>432</v>
       </c>
       <c r="F5">
-        <v>4176.09</v>
+        <v>4437.14</v>
       </c>
       <c r="G5">
-        <v>236.54</v>
+        <v>289.47</v>
       </c>
       <c r="H5">
-        <v>9846.68</v>
+        <v>9487.949999999999</v>
       </c>
     </row>
     <row r="6">
@@ -482,25 +482,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4050.65</v>
+        <v>4331.88</v>
       </c>
       <c r="C6">
-        <v>5364.06</v>
+        <v>5527.2</v>
       </c>
       <c r="D6">
-        <v>6219.7</v>
+        <v>6083.98</v>
       </c>
       <c r="E6">
-        <v>2880</v>
+        <v>432</v>
       </c>
       <c r="F6">
-        <v>9314.82</v>
+        <v>10224.64</v>
       </c>
       <c r="G6">
-        <v>2544.05</v>
+        <v>2599.44</v>
       </c>
       <c r="H6">
-        <v>30373.28</v>
+        <v>29199.139999999996</v>
       </c>
     </row>
     <row r="7">
@@ -508,25 +508,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9008.5</v>
+        <v>8164.8</v>
       </c>
       <c r="C7">
-        <v>12717.1</v>
+        <v>11322.69</v>
       </c>
       <c r="D7">
-        <v>13505.71</v>
+        <v>12906.9</v>
       </c>
       <c r="E7">
-        <v>8208</v>
+        <v>2160</v>
       </c>
       <c r="F7">
-        <v>28295.46</v>
+        <v>29066.32</v>
       </c>
       <c r="G7">
-        <v>10867.33</v>
+        <v>11761.73</v>
       </c>
       <c r="H7">
-        <v>82602.09999999999</v>
+        <v>75382.44</v>
       </c>
     </row>
     <row r="8">
@@ -534,25 +534,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>15018.7</v>
+        <v>14633.14</v>
       </c>
       <c r="C8">
-        <v>25170.56</v>
+        <v>25971.77</v>
       </c>
       <c r="D8">
-        <v>24512.35</v>
+        <v>24584.07</v>
       </c>
       <c r="E8">
-        <v>15408</v>
+        <v>5472</v>
       </c>
       <c r="F8">
-        <v>55222.37</v>
+        <v>59102.82</v>
       </c>
       <c r="G8">
-        <v>26899.83</v>
+        <v>28363.75</v>
       </c>
       <c r="H8">
-        <v>162231.81</v>
+        <v>158127.55000000002</v>
       </c>
     </row>
     <row r="9">
@@ -560,25 +560,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>16606.3</v>
+        <v>16270.63</v>
       </c>
       <c r="C9">
-        <v>36123.11</v>
+        <v>35951.54</v>
       </c>
       <c r="D9">
-        <v>31721.16</v>
+        <v>30924</v>
       </c>
       <c r="E9">
-        <v>11232</v>
+        <v>5328</v>
       </c>
       <c r="F9">
-        <v>40250.28</v>
+        <v>41854.59</v>
       </c>
       <c r="G9">
-        <v>15917.64</v>
+        <v>17046.15</v>
       </c>
       <c r="H9">
-        <v>151850.49</v>
+        <v>147374.91</v>
       </c>
     </row>
     <row r="10">
@@ -586,25 +586,25 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4517.86</v>
+        <v>4309.2</v>
       </c>
       <c r="C10">
-        <v>8356.41</v>
+        <v>8375.99</v>
       </c>
       <c r="D10">
-        <v>7850.71</v>
+        <v>7987.75</v>
       </c>
       <c r="E10">
-        <v>4608</v>
+        <v>1152</v>
       </c>
       <c r="F10">
-        <v>12048.05</v>
+        <v>11374.67</v>
       </c>
       <c r="G10">
-        <v>4313.06</v>
+        <v>3667.27</v>
       </c>
       <c r="H10">
-        <v>41694.09</v>
+        <v>36866.88</v>
       </c>
     </row>
     <row r="11">
@@ -612,25 +612,25 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2204.5</v>
+        <v>2159.14</v>
       </c>
       <c r="C11">
-        <v>3204.74</v>
+        <v>3700.21</v>
       </c>
       <c r="D11">
-        <v>3255.56</v>
+        <v>3570.17</v>
       </c>
       <c r="E11">
-        <v>2592</v>
+        <v>864</v>
       </c>
       <c r="F11">
-        <v>8182.5</v>
+        <v>6049.94</v>
       </c>
       <c r="G11">
-        <v>3546.09</v>
+        <v>2548.78</v>
       </c>
       <c r="H11">
-        <v>22985.39</v>
+        <v>18892.239999999998</v>
       </c>
     </row>
     <row r="12">
@@ -638,25 +638,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1800.79</v>
+        <v>1628.42</v>
       </c>
       <c r="C12">
-        <v>2263.76</v>
+        <v>2614.04</v>
       </c>
       <c r="D12">
-        <v>2931.5</v>
+        <v>2526.46</v>
       </c>
       <c r="E12">
-        <v>1872</v>
+        <v>144</v>
       </c>
       <c r="F12">
-        <v>7217.02</v>
+        <v>4622.61</v>
       </c>
       <c r="G12">
-        <v>3019.65</v>
+        <v>1480.87</v>
       </c>
       <c r="H12">
-        <v>19104.72</v>
+        <v>13016.399999999998</v>
       </c>
     </row>
     <row r="13">
@@ -664,25 +664,25 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2580.98</v>
+        <v>2503.87</v>
       </c>
       <c r="C13">
-        <v>4539.99</v>
+        <v>4118.1</v>
       </c>
       <c r="D13">
-        <v>5455.74</v>
+        <v>4727.63</v>
       </c>
       <c r="E13">
-        <v>2016</v>
+        <v>720</v>
       </c>
       <c r="F13">
-        <v>6646.87</v>
+        <v>4122.06</v>
       </c>
       <c r="G13">
-        <v>2378.11</v>
+        <v>786.04</v>
       </c>
       <c r="H13">
-        <v>23617.69</v>
+        <v>16977.7</v>
       </c>
     </row>
     <row r="14">
@@ -690,25 +690,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4871.66</v>
+        <v>4272.91</v>
       </c>
       <c r="C14">
-        <v>7113.67</v>
+        <v>6657.7</v>
       </c>
       <c r="D14">
-        <v>11492.46</v>
+        <v>11189.88</v>
       </c>
       <c r="E14">
-        <v>1584</v>
+        <v>432</v>
       </c>
       <c r="F14">
-        <v>6963.95</v>
+        <v>5179.66</v>
       </c>
       <c r="G14">
-        <v>880.97</v>
+        <v>552.49</v>
       </c>
       <c r="H14">
-        <v>32906.71</v>
+        <v>28284.64</v>
       </c>
     </row>
     <row r="15">
@@ -716,25 +716,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6418.44</v>
+        <v>6391.22</v>
       </c>
       <c r="C15">
-        <v>6161.92</v>
+        <v>5767.98</v>
       </c>
       <c r="D15">
-        <v>15481.28</v>
+        <v>15188.5</v>
       </c>
       <c r="E15">
-        <v>3600</v>
+        <v>864</v>
       </c>
       <c r="F15">
-        <v>12623.49</v>
+        <v>9357.3</v>
       </c>
       <c r="G15">
-        <v>276.55</v>
+        <v>185.13</v>
       </c>
       <c r="H15">
-        <v>44561.68</v>
+        <v>37754.13</v>
       </c>
     </row>
     <row r="16">
@@ -742,25 +742,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>7534.3</v>
+        <v>7702.13</v>
       </c>
       <c r="C16">
-        <v>6013.29</v>
+        <v>6155.52</v>
       </c>
       <c r="D16">
-        <v>14632.93</v>
+        <v>15685.31</v>
       </c>
       <c r="E16">
-        <v>5616</v>
+        <v>1584</v>
       </c>
       <c r="F16">
-        <v>21081.8</v>
+        <v>17784.25</v>
       </c>
       <c r="G16">
-        <v>73.8</v>
+        <v>150.1</v>
       </c>
       <c r="H16">
-        <v>54952.12000000001</v>
+        <v>49061.31</v>
       </c>
     </row>
     <row r="17">
@@ -768,25 +768,25 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>10605.17</v>
+        <v>10500.84</v>
       </c>
       <c r="C17">
-        <v>9073.84</v>
+        <v>9217.81</v>
       </c>
       <c r="D17">
-        <v>17398.37</v>
+        <v>16667.26</v>
       </c>
       <c r="E17">
-        <v>7200</v>
+        <v>1728</v>
       </c>
       <c r="F17">
-        <v>31602.04</v>
+        <v>30091.36</v>
       </c>
       <c r="G17">
-        <v>34.95</v>
+        <v>34.39</v>
       </c>
       <c r="H17">
-        <v>75914.37000000001</v>
+        <v>68239.66</v>
       </c>
     </row>
     <row r="18">
@@ -794,25 +794,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>12891.31</v>
+        <v>12836.88</v>
       </c>
       <c r="C18">
-        <v>11625.27</v>
+        <v>11381.7</v>
       </c>
       <c r="D18">
-        <v>16069.24</v>
+        <v>14356.91</v>
       </c>
       <c r="E18">
-        <v>12960</v>
+        <v>3312</v>
       </c>
       <c r="F18">
-        <v>43776.57</v>
+        <v>45621</v>
       </c>
       <c r="G18">
-        <v>4.02</v>
+        <v>13.42</v>
       </c>
       <c r="H18">
-        <v>97326.41</v>
+        <v>87521.91</v>
       </c>
     </row>
     <row r="19">
@@ -820,25 +820,25 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>14429.02</v>
+        <v>14909.83</v>
       </c>
       <c r="C19">
-        <v>13795.74</v>
+        <v>14494.58</v>
       </c>
       <c r="D19">
-        <v>12222.72</v>
+        <v>11755.61</v>
       </c>
       <c r="E19">
-        <v>13824</v>
+        <v>4320</v>
       </c>
       <c r="F19">
-        <v>53677.24</v>
+        <v>60054.78</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>107948.72</v>
+        <v>105534.8</v>
       </c>
     </row>
     <row r="20">
@@ -846,25 +846,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>17309.38</v>
+        <v>16697.02</v>
       </c>
       <c r="C20">
-        <v>24020.75</v>
+        <v>23225.98</v>
       </c>
       <c r="D20">
-        <v>14769.49</v>
+        <v>14902.16</v>
       </c>
       <c r="E20">
-        <v>14688</v>
+        <v>4320</v>
       </c>
       <c r="F20">
-        <v>63214.88</v>
+        <v>67508.29</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>134002.5</v>
+        <v>126653.45</v>
       </c>
     </row>
     <row r="21">
@@ -872,25 +872,25 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>16742.38</v>
+        <v>16361.35</v>
       </c>
       <c r="C21">
-        <v>19922.64</v>
+        <v>18145.71</v>
       </c>
       <c r="D21">
-        <v>13132.26</v>
+        <v>12150.66</v>
       </c>
       <c r="E21">
-        <v>13680</v>
+        <v>4320</v>
       </c>
       <c r="F21">
-        <v>66820.02</v>
+        <v>65763.73</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
-        <v>130297.30000000002</v>
+        <v>116741.45</v>
       </c>
     </row>
     <row r="22">
@@ -898,25 +898,25 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>14034.38</v>
+        <v>13653.36</v>
       </c>
       <c r="C22">
-        <v>13158.32</v>
+        <v>13465.59</v>
       </c>
       <c r="D22">
-        <v>11236.77</v>
+        <v>11924.95</v>
       </c>
       <c r="E22">
-        <v>12240</v>
+        <v>5040</v>
       </c>
       <c r="F22">
-        <v>57067.23</v>
+        <v>56300.88</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
-        <v>107736.70000000001</v>
+        <v>100384.78</v>
       </c>
     </row>
     <row r="23">
@@ -924,25 +924,25 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>11811.74</v>
+        <v>11984.11</v>
       </c>
       <c r="C23">
-        <v>9971.16</v>
+        <v>9547.84</v>
       </c>
       <c r="D23">
-        <v>15439.7</v>
+        <v>14809.43</v>
       </c>
       <c r="E23">
-        <v>11088</v>
+        <v>2880</v>
       </c>
       <c r="F23">
-        <v>43059.2</v>
+        <v>43801.83</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
-        <v>91369.8</v>
+        <v>83023.21</v>
       </c>
     </row>
     <row r="24">
@@ -950,25 +950,25 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>8754.48</v>
+        <v>8359.85</v>
       </c>
       <c r="C24">
-        <v>6805.22</v>
+        <v>6859.34</v>
       </c>
       <c r="D24">
-        <v>12912.41</v>
+        <v>12564.61</v>
       </c>
       <c r="E24">
-        <v>6192</v>
+        <v>2448</v>
       </c>
       <c r="F24">
-        <v>28358.69</v>
+        <v>26128.34</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>63022.8</v>
+        <v>56360.14</v>
       </c>
     </row>
     <row r="25">
@@ -976,25 +976,25 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>5574.74</v>
+        <v>5470.42</v>
       </c>
       <c r="C25">
-        <v>4652.18</v>
+        <v>4105.49</v>
       </c>
       <c r="D25">
-        <v>9918.42</v>
+        <v>9834.86</v>
       </c>
       <c r="E25">
-        <v>3888</v>
+        <v>1296</v>
       </c>
       <c r="F25">
-        <v>16438.54</v>
+        <v>13119.88</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>40471.880000000005</v>
+        <v>33826.65</v>
       </c>
     </row>
     <row r="26">
@@ -1002,25 +1002,25 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <v>192027.04</v>
+        <v>188194.10000000003</v>
       </c>
       <c r="C26">
-        <v>231441.74</v>
+        <v>227887.59999999998</v>
       </c>
       <c r="D26">
-        <v>261603.77</v>
+        <v>255913.73000000004</v>
       </c>
       <c r="E26">
-        <v>158688</v>
+        <v>49680</v>
       </c>
       <c r="F26">
-        <v>626838.7799999999</v>
+        <v>622493.8699999999</v>
       </c>
       <c r="G26">
-        <v>71007.19</v>
+        <v>69482.42</v>
       </c>
       <c r="H26">
-        <v>1541606.52</v>
+        <v>1413651.7199999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>